<commit_message>
deleted all, beginning of eval board
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\Stiftehalter\control_pcb\v3_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\sh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B634E0-167F-44C7-AF79-275CB07ADCCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585B44E9-DE4C-4CE5-8BCE-41AAFCFE0B1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
+    <workbookView xWindow="4620" yWindow="4530" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="V3.1" sheetId="1" r:id="rId1"/>
+    <sheet name="V3.2-evalboards" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="108">
   <si>
     <t>Bestellnummer</t>
   </si>
@@ -298,6 +299,66 @@
   </si>
   <si>
     <t>390 Ohm</t>
+  </si>
+  <si>
+    <t>micro usb</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TPD2E2U06DCKR?qs=xZ%2FP%252Ba9zWqa9UMTS1HgCWA%3D%3D</t>
+  </si>
+  <si>
+    <t>TPD2E2U06DCKR</t>
+  </si>
+  <si>
+    <t>595-TPD2E2U06DCKR</t>
+  </si>
+  <si>
+    <t>Lagerbestand</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV76733DGNR?qs=W%2FMpXkg%252BdQ7WCurh%2FfEdlw%3D%3D</t>
+  </si>
+  <si>
+    <t>3,3 Buck Regulator</t>
+  </si>
+  <si>
+    <t>TLV76733DGNR</t>
+  </si>
+  <si>
+    <t>595-TLV76733DGNR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TPS62237DRYR?qs=%2Fha2pyFadugVmGhGLsuKguvK6SvsWvP2nzaTTJxrA6tcgB4ILhcgJQ%3D%3D</t>
+  </si>
+  <si>
+    <t>buck_1</t>
+  </si>
+  <si>
+    <t>Buck_2</t>
+  </si>
+  <si>
+    <t>TPS62237DRYR</t>
+  </si>
+  <si>
+    <t>595-TPS62237DRYR</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TPS73533DRBT?qs=IDSsxkoac0yHZOHlDK7%252B5A%3D%3D</t>
+  </si>
+  <si>
+    <t>TPS73533DRBT</t>
+  </si>
+  <si>
+    <t>595-TPS73533DRBT</t>
   </si>
 </sst>
 </file>
@@ -678,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B41CD6A-5D50-4B39-8AD6-0D352983D4FC}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,4 +1104,150 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B617D8-6A84-417E-865C-A831196F2879}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{80451E08-9130-4852-B7FF-E2FAB0B95011}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
split in two boards from now on
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\sh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3045EB7-85C1-4A24-A953-36261F6A36CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D6205D-319A-45ED-9E9D-15FE6EEDF2AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="4530" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
+    <workbookView xWindow="-23520" yWindow="3765" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
   </bookViews>
   <sheets>
     <sheet name="V3.1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="128">
   <si>
     <t>Bestellnummer</t>
   </si>
@@ -310,9 +310,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV76733DGNR?qs=W%2FMpXkg%252BdQ7WCurh%2FfEdlw%3D%3D</t>
   </si>
   <si>
@@ -325,21 +322,9 @@
     <t>595-TLV76733DGNR</t>
   </si>
   <si>
-    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TPS62237DRYR?qs=%2Fha2pyFadugVmGhGLsuKguvK6SvsWvP2nzaTTJxrA6tcgB4ILhcgJQ%3D%3D</t>
-  </si>
-  <si>
     <t>buck_1</t>
   </si>
   <si>
-    <t>Buck_2</t>
-  </si>
-  <si>
-    <t>TPS62237DRYR</t>
-  </si>
-  <si>
-    <t>595-TPS62237DRYR</t>
-  </si>
-  <si>
     <t>LDO</t>
   </si>
   <si>
@@ -352,15 +337,6 @@
     <t>595-TPS73533DRBT</t>
   </si>
   <si>
-    <t>https://www.mouser.de/ProductDetail/ON-Semiconductor/1N4002RLG?qs=y2kkmE52mdMfmlxIpNIwcg%3D%3D</t>
-  </si>
-  <si>
-    <t>863-1N4002RLG</t>
-  </si>
-  <si>
-    <t>1N4002RLG</t>
-  </si>
-  <si>
     <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TPS2044BDR?qs=ojKcPFmCWSWjSLiA1%252Bod3Q%3D%3D</t>
   </si>
   <si>
@@ -373,18 +349,6 @@
     <t>595-TPS2044BDR</t>
   </si>
   <si>
-    <t>https://www.mouser.de/ProductDetail/Wurth-Elektronik/885012208043?qs=0KOYDY2FL2%252BcdWD1v8wtpw%3D%3D</t>
-  </si>
-  <si>
-    <t>330pF</t>
-  </si>
-  <si>
-    <t>710-885012208043</t>
-  </si>
-  <si>
-    <t>885012208043</t>
-  </si>
-  <si>
     <t>https://www.mouser.de/ProductDetail/Texas-Instruments/SN75240PW?qs=q2XTDbzbm6CHHo1l5fz%2Fyw%3D%3D</t>
   </si>
   <si>
@@ -392,6 +356,69 @@
   </si>
   <si>
     <t>595-SN75240PW</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>UMA1V2R2MCD2</t>
+  </si>
+  <si>
+    <t>647-UMA1V2R2MCD2</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Nichicon/UMA1V2R2MCD2?qs=sGAEpiMZZMsh%252B1woXyUXj6bDod02pHYQR6QR3MfcWjw%3D</t>
+  </si>
+  <si>
+    <t>UMA1E4R7MDD</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>647-UMA1E4R7MDD</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Nichicon/UMA1E4R7MDD?qs=sGAEpiMZZMsh%252B1woXyUXj6YRc%252B4zXg5f1UnAAA5WZao%3D</t>
+  </si>
+  <si>
+    <t>1N4002-E3/54</t>
+  </si>
+  <si>
+    <t>625-1N4002-E3/54</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Vishay-General-Semiconductor/1N4002-E3-54?qs=N4vtoAxH%2FSqs13dJhGS5gw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Molex/105017-0001?qs=sGAEpiMZZMvlX3nhDDO4AA0VO14TO52rzX8fMMJntC8%3D</t>
+  </si>
+  <si>
+    <t>105017-0001</t>
+  </si>
+  <si>
+    <t>538-105017-0001</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Molex/67643-0910?qs=EuyFtE1skifNhj6pwWTsXw%3D%3D</t>
+  </si>
+  <si>
+    <t>usb a</t>
+  </si>
+  <si>
+    <t>67643-0910</t>
+  </si>
+  <si>
+    <t>538-67643-0910</t>
+  </si>
+  <si>
+    <t>usb hub</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TUSB2046IBVF?qs=HXFqYaX1Q2zoacj5Hiwo4Q%3D%3D</t>
+  </si>
+  <si>
+    <t>green</t>
   </si>
 </sst>
 </file>
@@ -429,12 +456,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -450,12 +483,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1142,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B617D8-6A84-417E-865C-A831196F2879}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,156 +1213,192 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
+      <c r="A2" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>88</v>
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="F3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
+      <c r="A4" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>115</v>
+      <c r="A10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>112</v>
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" xr:uid="{80451E08-9130-4852-B7FF-E2FAB0B95011}"/>
-    <hyperlink ref="E10" r:id="rId2" xr:uid="{470705F8-3988-43D5-83DB-0A53AEF5DAB4}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{C673DB03-5B45-4C25-A2B9-8ED25ABB1025}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{80451E08-9130-4852-B7FF-E2FAB0B95011}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{C673DB03-5B45-4C25-A2B9-8ED25ABB1025}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{8E085EE2-2646-4FC3-A262-5DB2BC28D809}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{D1CB7C2E-21EA-4053-95DD-C083042A72EA}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{8B6D4956-3F10-4801-8347-DBF104FE2B36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new branch, only for usb hub
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\sh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D6205D-319A-45ED-9E9D-15FE6EEDF2AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A8F19C-3FFB-47CA-A6B0-FCC2F8A9E4DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23520" yWindow="3765" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
+    <workbookView xWindow="4635" yWindow="5175" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
   </bookViews>
   <sheets>
     <sheet name="V3.1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
   <si>
     <t>Bestellnummer</t>
   </si>
@@ -1176,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B617D8-6A84-417E-865C-A831196F2879}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,6 +1390,11 @@
         <v>66</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{80451E08-9130-4852-B7FF-E2FAB0B95011}"/>

</xml_diff>

<commit_message>
review passed, bom created
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\sh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A8F19C-3FFB-47CA-A6B0-FCC2F8A9E4DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B525D525-E753-48D4-AEAD-7A058ADAC908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="5175" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
   </bookViews>
   <sheets>
     <sheet name="V3.1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="132">
   <si>
     <t>Bestellnummer</t>
   </si>
@@ -419,6 +419,18 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/TE-Connectivity-Alcoswitch/FSM4JH?qs=g%252BEszo6zu8OwVWrHD2r3Rw==</t>
+  </si>
+  <si>
+    <t>FSM4JH</t>
+  </si>
+  <si>
+    <t>506-FSM4JH</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1191,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1404,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>67</v>
+        <v>128</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new project for atmgea evalboard
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\sh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAFD017-72B8-4395-AA4E-21ED13965C3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106C43AB-4918-4F5B-BC18-5A3F89C6EB3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{48259633-EE13-4C27-8187-B057E0959B49}"/>
   </bookViews>
   <sheets>
     <sheet name="V3.1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="134">
   <si>
     <t>Bestellnummer</t>
   </si>
@@ -420,6 +420,24 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Amphenol-FCI/20021111-00016T4LF?qs=nwYJ12Fl9gTdul0SmoJcyA%3D%3D</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>2*8</t>
+  </si>
+  <si>
+    <t>20021111-00016T4LF</t>
+  </si>
+  <si>
+    <t>649-221111-00016T4LF</t>
+  </si>
+  <si>
+    <t>Fuse</t>
   </si>
 </sst>
 </file>
@@ -457,7 +475,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,6 +485,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,13 +508,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1180,7 +1205,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,14 +1431,64 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5536883-80AF-4B37-945B-A42087A37304}">
-  <dimension ref="A1"/>
+  <dimension ref="A4:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="104.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>